<commit_message>
Estado de Avance al 29 de Agosto de 2014
Se actualizaron documentos del Estado de Avance al 29 de Agosto de 2014
</commit_message>
<xml_diff>
--- a/doc/0.1.0/Desempeño del proceso 2013-09.xlsx
+++ b/doc/0.1.0/Desempeño del proceso 2013-09.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodrigo.esparza\Documentos\GitHub\LMEC\doc\0.1.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="15120" windowHeight="7995" activeTab="1"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LMEC!$A$1:$M$275</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -294,10 +299,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -311,6 +316,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -318,7 +326,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -390,6 +398,13 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -397,6 +412,12 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -438,6 +459,13 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -445,6 +473,12 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -480,21 +514,22 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="90758144"/>
-        <c:axId val="60778176"/>
+        <c:axId val="233442656"/>
+        <c:axId val="233443048"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="90758144"/>
+        <c:axId val="233442656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60778176"/>
+        <c:crossAx val="233443048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -502,7 +537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60778176"/>
+        <c:axId val="233443048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +553,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="90758144"/>
+        <c:crossAx val="233442656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -543,7 +578,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -634,21 +669,22 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="109535744"/>
-        <c:axId val="60780480"/>
+        <c:axId val="233443832"/>
+        <c:axId val="233444224"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="109535744"/>
+        <c:axId val="233443832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60780480"/>
+        <c:crossAx val="233444224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -656,7 +692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60780480"/>
+        <c:axId val="233444224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,7 +703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109535744"/>
+        <c:crossAx val="233443832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -692,7 +728,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -766,6 +802,28 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>LMEC!$E$4:$E$12</c:f>
@@ -853,6 +911,28 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>LMEC!$E$4:$E$12</c:f>
@@ -936,21 +1016,22 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="109537280"/>
-        <c:axId val="60782208"/>
+        <c:axId val="233445008"/>
+        <c:axId val="233445400"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="109537280"/>
+        <c:axId val="233445008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60782208"/>
+        <c:crossAx val="233445400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -958,7 +1039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60782208"/>
+        <c:axId val="233445400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +1049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109537280"/>
+        <c:crossAx val="233445008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -993,7 +1074,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1013,7 +1094,6 @@
       <c:rotX val="30"/>
       <c:rotY val="0"/>
       <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -1043,6 +1123,13 @@
             </c:strRef>
           </c:tx>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1050,6 +1137,11 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1158,13 +1250,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1326,7 +1418,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1361,7 +1453,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1572,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N205"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2591,7 @@
   <dimension ref="A1:N430"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,7 +2618,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="3">
@@ -2546,7 +2638,7 @@
       <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="3">
         <v>41088</v>
       </c>
@@ -2582,7 +2674,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="3">
         <v>41089</v>
       </c>
@@ -2625,7 +2717,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3">
         <v>41092</v>
       </c>
@@ -2668,7 +2760,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3">
         <v>41093</v>
       </c>
@@ -2711,7 +2803,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="3">
         <v>41094</v>
       </c>
@@ -2754,7 +2846,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="3">
         <v>41095</v>
       </c>
@@ -2797,7 +2889,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="3">
         <v>41096</v>
       </c>
@@ -2840,7 +2932,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="3">
         <v>41099</v>
       </c>
@@ -2883,7 +2975,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3">
         <v>41100</v>
       </c>
@@ -2926,7 +3018,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="3">
         <v>41101</v>
       </c>
@@ -2969,7 +3061,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="3">
         <v>41102</v>
       </c>
@@ -3011,13 +3103,13 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="3">
         <v>41103</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="3">
         <v>41127</v>
       </c>
@@ -3035,7 +3127,7 @@
       <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="3">
         <v>41128</v>
       </c>
@@ -3071,7 +3163,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="3">
         <v>41129</v>
       </c>
@@ -3116,7 +3208,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="3">
         <v>41130</v>
       </c>
@@ -3124,13 +3216,13 @@
       <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="3">
         <v>41131</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="3">
@@ -3138,61 +3230,61 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="3">
         <v>41135</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="3">
         <v>41136</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="3">
         <v>41137</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="3">
         <v>41138</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="3">
         <v>41141</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="3">
         <v>41142</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="3">
         <v>41143</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="3">
         <v>41144</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="3">
         <v>41145</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="3">
@@ -3200,151 +3292,151 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="3">
         <v>41149</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="3">
         <v>41150</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="3">
         <v>41151</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="3">
         <v>41152</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="3">
         <v>41155</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="3">
         <v>41156</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="3">
         <v>41157</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="3">
         <v>41158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="3">
         <v>41159</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="3">
         <v>41162</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="3">
         <v>41163</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="3">
         <v>41164</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="3">
         <v>41165</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="3">
         <v>41166</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="3">
         <v>41169</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="3">
         <v>41170</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="3">
         <v>41171</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="3">
         <v>41172</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="3">
         <v>41173</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="3">
         <v>41176</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="3">
         <v>41177</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="3">
         <v>41178</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="3">
         <v>41179</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="3">
         <v>41180</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="3">
@@ -3352,787 +3444,787 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="3">
         <v>41184</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="3">
         <v>41185</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="3">
         <v>41186</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="3">
         <v>41187</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="3">
         <v>41190</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="3">
         <v>41191</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="3">
         <v>41192</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="3">
         <v>41193</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="3">
         <v>41197</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="3">
         <v>41198</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="3">
         <v>41199</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="3">
         <v>41200</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="3">
         <v>41201</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
+      <c r="A69" s="21"/>
       <c r="B69" s="3">
         <v>41204</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="3">
         <v>41205</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="3">
         <v>41206</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="3">
         <v>41207</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="3">
         <v>41208</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="3">
         <v>41211</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="20"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="3">
         <v>41212</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="3">
         <v>41213</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
+      <c r="A77" s="21"/>
       <c r="B77" s="3">
         <v>41218</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="20"/>
+      <c r="A78" s="21"/>
       <c r="B78" s="3">
         <v>41219</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
+      <c r="A79" s="21"/>
       <c r="B79" s="3">
         <v>41220</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="20"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="3">
         <v>41221</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="20"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="3">
         <v>41222</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="3">
         <v>41225</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
+      <c r="A83" s="21"/>
       <c r="B83" s="3">
         <v>41226</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="3">
         <v>41227</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="3">
         <v>41228</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="20"/>
+      <c r="A86" s="21"/>
       <c r="B86" s="3">
         <v>41229</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="20"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="3">
         <v>41233</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="20"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="3">
         <v>41234</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="20"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="3">
         <v>41235</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="20"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="3">
         <v>41236</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="20"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="3">
         <v>41239</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
+      <c r="A92" s="21"/>
       <c r="B92" s="3">
         <v>41240</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="3">
         <v>41241</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="20"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="3">
         <v>41242</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="20"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="3">
         <v>41243</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="20"/>
+      <c r="A96" s="21"/>
       <c r="B96" s="3">
         <v>41246</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="20"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="3">
         <v>41247</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="20"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="3">
         <v>41248</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="20"/>
+      <c r="A99" s="21"/>
       <c r="B99" s="3">
         <v>41249</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="20"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="3">
         <v>41250</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="20"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="3">
         <v>41253</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="20"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="3">
         <v>41254</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="20"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="3">
         <v>41255</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="20"/>
+      <c r="A104" s="21"/>
       <c r="B104" s="3">
         <v>41256</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="20"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="3">
         <v>41257</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="20"/>
+      <c r="A106" s="21"/>
       <c r="B106" s="3">
         <v>41260</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="20"/>
+      <c r="A107" s="21"/>
       <c r="B107" s="3">
         <v>41261</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="20"/>
+      <c r="A108" s="21"/>
       <c r="B108" s="3">
         <v>41281</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="20"/>
+      <c r="A109" s="21"/>
       <c r="B109" s="3">
         <v>41282</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="20"/>
+      <c r="A110" s="21"/>
       <c r="B110" s="3">
         <v>41283</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="20"/>
+      <c r="A111" s="21"/>
       <c r="B111" s="3">
         <v>41284</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="20"/>
+      <c r="A112" s="21"/>
       <c r="B112" s="3">
         <v>41285</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="20"/>
+      <c r="A113" s="21"/>
       <c r="B113" s="3">
         <v>41288</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
+      <c r="A114" s="21"/>
       <c r="B114" s="3">
         <v>41289</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
+      <c r="A115" s="21"/>
       <c r="B115" s="3">
         <v>41290</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="20"/>
+      <c r="A116" s="21"/>
       <c r="B116" s="3">
         <v>41291</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="20"/>
+      <c r="A117" s="21"/>
       <c r="B117" s="3">
         <v>41292</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="20"/>
+      <c r="A118" s="21"/>
       <c r="B118" s="3">
         <v>41295</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="20"/>
+      <c r="A119" s="21"/>
       <c r="B119" s="3">
         <v>41296</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="20"/>
+      <c r="A120" s="21"/>
       <c r="B120" s="3">
         <v>41297</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="20"/>
+      <c r="A121" s="21"/>
       <c r="B121" s="3">
         <v>41298</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="20"/>
+      <c r="A122" s="21"/>
       <c r="B122" s="3">
         <v>41299</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="20"/>
+      <c r="A123" s="21"/>
       <c r="B123" s="3">
         <v>41302</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="20"/>
+      <c r="A124" s="21"/>
       <c r="B124" s="3">
         <v>41303</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="20"/>
+      <c r="A125" s="21"/>
       <c r="B125" s="3">
         <v>41304</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="20"/>
+      <c r="A126" s="21"/>
       <c r="B126" s="3">
         <v>41305</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="20"/>
+      <c r="A127" s="21"/>
       <c r="B127" s="3">
         <v>41306</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="20"/>
+      <c r="A128" s="21"/>
       <c r="B128" s="3">
         <v>41310</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="20"/>
+      <c r="A129" s="21"/>
       <c r="B129" s="3">
         <v>41311</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="20"/>
+      <c r="A130" s="21"/>
       <c r="B130" s="3">
         <v>41312</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="20"/>
+      <c r="A131" s="21"/>
       <c r="B131" s="3">
         <v>41313</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="20"/>
+      <c r="A132" s="21"/>
       <c r="B132" s="3">
         <v>41318</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="20"/>
+      <c r="A133" s="21"/>
       <c r="B133" s="3">
         <v>41319</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="20"/>
+      <c r="A134" s="21"/>
       <c r="B134" s="3">
         <v>41320</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="20"/>
+      <c r="A135" s="21"/>
       <c r="B135" s="3">
         <v>41323</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="20"/>
+      <c r="A136" s="21"/>
       <c r="B136" s="3">
         <v>41324</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="20"/>
+      <c r="A137" s="21"/>
       <c r="B137" s="3">
         <v>41325</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="20"/>
+      <c r="A138" s="21"/>
       <c r="B138" s="3">
         <v>41326</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="20"/>
+      <c r="A139" s="21"/>
       <c r="B139" s="3">
         <v>41327</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="20"/>
+      <c r="A140" s="21"/>
       <c r="B140" s="3">
         <v>41331</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="20"/>
+      <c r="A141" s="21"/>
       <c r="B141" s="3">
         <v>41332</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="20"/>
+      <c r="A142" s="21"/>
       <c r="B142" s="3">
         <v>41333</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="20"/>
+      <c r="A143" s="21"/>
       <c r="B143" s="3">
         <v>41334</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="20"/>
+      <c r="A144" s="21"/>
       <c r="B144" s="3">
         <v>41337</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="20"/>
+      <c r="A145" s="21"/>
       <c r="B145" s="3">
         <v>41338</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="20"/>
+      <c r="A146" s="21"/>
       <c r="B146" s="3">
         <v>41339</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="20"/>
+      <c r="A147" s="21"/>
       <c r="B147" s="3">
         <v>41340</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="20"/>
+      <c r="A148" s="21"/>
       <c r="B148" s="3">
         <v>41341</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="20"/>
+      <c r="A149" s="21"/>
       <c r="B149" s="3">
         <v>41344</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="20"/>
+      <c r="A150" s="21"/>
       <c r="B150" s="3">
         <v>41345</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="20"/>
+      <c r="A151" s="21"/>
       <c r="B151" s="3">
         <v>41346</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="20"/>
+      <c r="A152" s="21"/>
       <c r="B152" s="3">
         <v>41347</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="20"/>
+      <c r="A153" s="21"/>
       <c r="B153" s="3">
         <v>41348</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="20"/>
+      <c r="A154" s="21"/>
       <c r="B154" s="3">
         <v>41352</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="20"/>
+      <c r="A155" s="21"/>
       <c r="B155" s="3">
         <v>41353</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="20"/>
+      <c r="A156" s="21"/>
       <c r="B156" s="3">
         <v>41354</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="20"/>
+      <c r="A157" s="21"/>
       <c r="B157" s="3">
         <v>41355</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="20"/>
+      <c r="A158" s="21"/>
       <c r="B158" s="3">
         <v>41372</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="20"/>
+      <c r="A159" s="21"/>
       <c r="B159" s="3">
         <v>41373</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="20"/>
+      <c r="A160" s="21"/>
       <c r="B160" s="3">
         <v>41374</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="20"/>
+      <c r="A161" s="21"/>
       <c r="B161" s="3">
         <v>41375</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="20"/>
+      <c r="A162" s="21"/>
       <c r="B162" s="3">
         <v>41376</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="20"/>
+      <c r="A163" s="21"/>
       <c r="B163" s="3">
         <v>41379</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="20"/>
+      <c r="A164" s="21"/>
       <c r="B164" s="3">
         <v>41380</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="20"/>
+      <c r="A165" s="21"/>
       <c r="B165" s="3">
         <v>41381</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="20"/>
+      <c r="A166" s="21"/>
       <c r="B166" s="3">
         <v>41382</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="20"/>
+      <c r="A167" s="21"/>
       <c r="B167" s="3">
         <v>41383</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="20"/>
+      <c r="A168" s="21"/>
       <c r="B168" s="3">
         <v>41386</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="20"/>
+      <c r="A169" s="21"/>
       <c r="B169" s="3">
         <v>41387</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="20"/>
+      <c r="A170" s="21"/>
       <c r="B170" s="3">
         <v>41388</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="20"/>
+      <c r="A171" s="21"/>
       <c r="B171" s="3">
         <v>41390</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="20"/>
+      <c r="A172" s="21"/>
       <c r="B172" s="3">
         <v>41393</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="20"/>
+      <c r="A173" s="21"/>
       <c r="B173" s="3">
         <v>41394</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="20"/>
+      <c r="A174" s="21"/>
       <c r="B174" s="3">
         <v>41396</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="20"/>
+      <c r="A175" s="21"/>
       <c r="B175" s="3">
         <v>41397</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="20"/>
+      <c r="A176" s="21"/>
       <c r="B176" s="3">
         <v>41400</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="20"/>
+      <c r="A177" s="21"/>
       <c r="B177" s="3">
         <v>41401</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="20"/>
+      <c r="A178" s="21"/>
       <c r="B178" s="3">
         <v>41402</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="20"/>
+      <c r="A179" s="21"/>
       <c r="B179" s="3">
         <v>41403</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="20"/>
+      <c r="A180" s="21"/>
       <c r="B180" s="3">
         <v>41407</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="20"/>
+      <c r="A181" s="21"/>
       <c r="B181" s="3">
         <v>41408</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="20"/>
+      <c r="A182" s="21"/>
       <c r="B182" s="3">
         <v>41410</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="20"/>
+      <c r="A183" s="21"/>
       <c r="B183" s="3">
         <v>41411</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="20"/>
+      <c r="A184" s="21"/>
       <c r="B184" s="3">
         <v>41414</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="20"/>
+      <c r="A185" s="21"/>
       <c r="B185" s="3">
         <v>41415</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="21" t="s">
+      <c r="A186" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B186" s="3">
@@ -4140,271 +4232,271 @@
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="21"/>
+      <c r="A187" s="20"/>
       <c r="B187" s="3">
         <v>41417</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="21"/>
+      <c r="A188" s="20"/>
       <c r="B188" s="3">
         <v>41418</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="21"/>
+      <c r="A189" s="20"/>
       <c r="B189" s="3">
         <v>41421</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="21"/>
+      <c r="A190" s="20"/>
       <c r="B190" s="3">
         <v>41422</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="21"/>
+      <c r="A191" s="20"/>
       <c r="B191" s="3">
         <v>41423</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="21"/>
+      <c r="A192" s="20"/>
       <c r="B192" s="3">
         <v>41424</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="21"/>
+      <c r="A193" s="20"/>
       <c r="B193" s="3">
         <v>41425</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="21"/>
+      <c r="A194" s="20"/>
       <c r="B194" s="3">
         <v>41428</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="21"/>
+      <c r="A195" s="20"/>
       <c r="B195" s="3">
         <v>41429</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="21"/>
+      <c r="A196" s="20"/>
       <c r="B196" s="3">
         <v>41430</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="21"/>
+      <c r="A197" s="20"/>
       <c r="B197" s="3">
         <v>41431</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="21"/>
+      <c r="A198" s="20"/>
       <c r="B198" s="3">
         <v>41432</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="21"/>
+      <c r="A199" s="20"/>
       <c r="B199" s="3">
         <v>41435</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="21"/>
+      <c r="A200" s="20"/>
       <c r="B200" s="3">
         <v>41436</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="21"/>
+      <c r="A201" s="20"/>
       <c r="B201" s="3">
         <v>41437</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="21"/>
+      <c r="A202" s="20"/>
       <c r="B202" s="3">
         <v>41438</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="21"/>
+      <c r="A203" s="20"/>
       <c r="B203" s="3">
         <v>41439</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="21"/>
+      <c r="A204" s="20"/>
       <c r="B204" s="3">
         <v>41442</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="21"/>
+      <c r="A205" s="20"/>
       <c r="B205" s="3">
         <v>41443</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="21"/>
+      <c r="A206" s="20"/>
       <c r="B206" s="3">
         <v>41444</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="21"/>
+      <c r="A207" s="20"/>
       <c r="B207" s="3">
         <v>41445</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="21"/>
+      <c r="A208" s="20"/>
       <c r="B208" s="3">
         <v>41446</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="21"/>
+      <c r="A209" s="20"/>
       <c r="B209" s="3">
         <v>41449</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="21"/>
+      <c r="A210" s="20"/>
       <c r="B210" s="3">
         <v>41450</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="21"/>
+      <c r="A211" s="20"/>
       <c r="B211" s="3">
         <v>41451</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="21"/>
+      <c r="A212" s="20"/>
       <c r="B212" s="3">
         <v>41452</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="21"/>
+      <c r="A213" s="20"/>
       <c r="B213" s="3">
         <v>41453</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="21"/>
+      <c r="A214" s="20"/>
       <c r="B214" s="3">
         <v>41456</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="21"/>
+      <c r="A215" s="20"/>
       <c r="B215" s="3">
         <v>41457</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="21"/>
+      <c r="A216" s="20"/>
       <c r="B216" s="3">
         <v>41458</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="21"/>
+      <c r="A217" s="20"/>
       <c r="B217" s="3">
         <v>41459</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="21"/>
+      <c r="A218" s="20"/>
       <c r="B218" s="3">
         <v>41460</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="21"/>
+      <c r="A219" s="20"/>
       <c r="B219" s="3">
         <v>41463</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="21"/>
+      <c r="A220" s="20"/>
       <c r="B220" s="3">
         <v>41464</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="21"/>
+      <c r="A221" s="20"/>
       <c r="B221" s="3">
         <v>41465</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="21"/>
+      <c r="A222" s="20"/>
       <c r="B222" s="3">
         <v>41466</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="21"/>
+      <c r="A223" s="20"/>
       <c r="B223" s="3">
         <v>41467</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="21"/>
+      <c r="A224" s="20"/>
       <c r="B224" s="3">
         <v>41470</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="21"/>
+      <c r="A225" s="20"/>
       <c r="B225" s="3">
         <v>41471</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="21"/>
+      <c r="A226" s="20"/>
       <c r="B226" s="3">
         <v>41493</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="21"/>
+      <c r="A227" s="20"/>
       <c r="B227" s="3">
         <v>41494</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="21"/>
+      <c r="A228" s="20"/>
       <c r="B228" s="3">
         <v>41495</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="21"/>
+      <c r="A229" s="20"/>
       <c r="B229" s="3">
         <v>41498</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="21"/>
+      <c r="A230" s="20"/>
       <c r="B230" s="3">
         <v>41499</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="21" t="s">
+      <c r="A231" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B231" s="3">
@@ -4412,121 +4504,121 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="21"/>
+      <c r="A232" s="20"/>
       <c r="B232" s="3">
         <v>41501</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="21"/>
+      <c r="A233" s="20"/>
       <c r="B233" s="3">
         <v>41502</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="21"/>
+      <c r="A234" s="20"/>
       <c r="B234" s="3">
         <v>41505</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="21"/>
+      <c r="A235" s="20"/>
       <c r="B235" s="3">
         <v>41506</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="21"/>
+      <c r="A236" s="20"/>
       <c r="B236" s="3">
         <v>41507</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="21"/>
+      <c r="A237" s="20"/>
       <c r="B237" s="3">
         <v>41508</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="21"/>
+      <c r="A238" s="20"/>
       <c r="B238" s="3">
         <v>41509</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="21"/>
+      <c r="A239" s="20"/>
       <c r="B239" s="3">
         <v>41512</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="21"/>
+      <c r="A240" s="20"/>
       <c r="B240" s="3">
         <v>41513</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="21"/>
+      <c r="A241" s="20"/>
       <c r="B241" s="3">
         <v>41514</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="21"/>
+      <c r="A242" s="20"/>
       <c r="B242" s="3">
         <v>41515</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="21"/>
+      <c r="A243" s="20"/>
       <c r="B243" s="3">
         <v>41516</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="21"/>
+      <c r="A244" s="20"/>
       <c r="B244" s="3">
         <v>41519</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="21"/>
+      <c r="A245" s="20"/>
       <c r="B245" s="3">
         <v>41520</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="21"/>
+      <c r="A246" s="20"/>
       <c r="B246" s="3">
         <v>41521</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="21"/>
+      <c r="A247" s="20"/>
       <c r="B247" s="3">
         <v>41522</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="21"/>
+      <c r="A248" s="20"/>
       <c r="B248" s="3">
         <v>41523</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="21"/>
+      <c r="A249" s="20"/>
       <c r="B249" s="3">
         <v>41526</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="21"/>
+      <c r="A250" s="20"/>
       <c r="B250" s="3">
         <v>41527</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="21" t="s">
+      <c r="A251" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B251" s="3">
@@ -4534,91 +4626,91 @@
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="21"/>
+      <c r="A252" s="20"/>
       <c r="B252" s="3">
         <v>41529</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="21"/>
+      <c r="A253" s="20"/>
       <c r="B253" s="3">
         <v>41530</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="21"/>
+      <c r="A254" s="20"/>
       <c r="B254" s="3">
         <v>41534</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="21"/>
+      <c r="A255" s="20"/>
       <c r="B255" s="3">
         <v>41535</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="21"/>
+      <c r="A256" s="20"/>
       <c r="B256" s="3">
         <v>41536</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="21"/>
+      <c r="A257" s="20"/>
       <c r="B257" s="3">
         <v>41537</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="21"/>
+      <c r="A258" s="20"/>
       <c r="B258" s="3">
         <v>41540</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="21"/>
+      <c r="A259" s="20"/>
       <c r="B259" s="3">
         <v>41541</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="21"/>
+      <c r="A260" s="20"/>
       <c r="B260" s="3">
         <v>41542</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="21"/>
+      <c r="A261" s="20"/>
       <c r="B261" s="3">
         <v>41543</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="21"/>
+      <c r="A262" s="20"/>
       <c r="B262" s="3">
         <v>41544</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="21"/>
+      <c r="A263" s="20"/>
       <c r="B263" s="3">
         <v>41547</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="21"/>
+      <c r="A264" s="20"/>
       <c r="B264" s="3">
         <v>41548</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="21"/>
+      <c r="A265" s="20"/>
       <c r="B265" s="3">
         <v>41549</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="21" t="s">
+      <c r="A266" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B266" s="3">
@@ -4626,31 +4718,31 @@
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="21"/>
+      <c r="A267" s="20"/>
       <c r="B267" s="3">
         <v>41551</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="21"/>
+      <c r="A268" s="20"/>
       <c r="B268" s="3">
         <v>41554</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="21"/>
+      <c r="A269" s="20"/>
       <c r="B269" s="3">
         <v>41555</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="21"/>
+      <c r="A270" s="20"/>
       <c r="B270" s="3">
         <v>41556</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="21" t="s">
+      <c r="A271" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B271" s="3">
@@ -4658,13 +4750,13 @@
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="21"/>
+      <c r="A272" s="20"/>
       <c r="B272" s="3">
         <v>41558</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="21"/>
+      <c r="A273" s="20"/>
       <c r="B273" s="3">
         <v>41561</v>
       </c>
@@ -5456,17 +5548,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A186:A230"/>
-    <mergeCell ref="A231:A250"/>
-    <mergeCell ref="A251:A265"/>
-    <mergeCell ref="A266:A270"/>
-    <mergeCell ref="A271:A273"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A20:A29"/>
     <mergeCell ref="A30:A54"/>
     <mergeCell ref="A55:A185"/>
     <mergeCell ref="D2:M2"/>
     <mergeCell ref="E15:N15"/>
+    <mergeCell ref="A186:A230"/>
+    <mergeCell ref="A231:A250"/>
+    <mergeCell ref="A251:A265"/>
+    <mergeCell ref="A266:A270"/>
+    <mergeCell ref="A271:A273"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>